<commit_message>
update on excel file
</commit_message>
<xml_diff>
--- a/ProjetFinal.xlsx
+++ b/ProjetFinal.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Conditions initiale et traj" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulation en mouvement" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +19,80 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Paramètre généraux                                                                                     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio constante d'Aaresth              </t>
+  </si>
+  <si>
+    <t>seconde</t>
+  </si>
+  <si>
+    <t>mètre/seconde</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Corps en mouvement</t>
+  </si>
+  <si>
+    <t>Masse</t>
+  </si>
+  <si>
+    <t>Accélération initiale</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Vitesse initiale</t>
+  </si>
+  <si>
+    <t>coefficient de friction                                                                           f</t>
+  </si>
+  <si>
+    <t>gramme</t>
+  </si>
+  <si>
+    <t>mètre</t>
+  </si>
+  <si>
+    <t>mètre/seconde²</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base de temps                                                                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                                                                  </t>
+  </si>
+  <si>
+    <t>Position initiale</t>
+  </si>
+  <si>
+    <t>La Terre</t>
+  </si>
+  <si>
+    <t>Mars</t>
+  </si>
+  <si>
+    <t>Trois corps statiques</t>
+  </si>
+  <si>
+    <t>Saturne</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +100,122 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="5" tint="-0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="9" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <bgColor theme="4" tint="-0.24994659260841701"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="darkGray">
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD3A663"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor theme="6" tint="-0.24994659260841701"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -45,18 +223,211 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2">
+      <alignment horizontal="left"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="3" borderId="2" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="7"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="8" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="5" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="9">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="9">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="10">
+    <cellStyle name="Données mars" xfId="7"/>
+    <cellStyle name="Données tableau" xfId="2"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Normal2" xfId="4"/>
+    <cellStyle name="Saturne" xfId="8"/>
+    <cellStyle name="Saturne titre données" xfId="9"/>
+    <cellStyle name="Titre corps2" xfId="5"/>
+    <cellStyle name="Titre données" xfId="3"/>
+    <cellStyle name="Titre données Mars" xfId="6"/>
+    <cellStyle name="titre table" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD3A663"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -69,7 +440,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -114,7 +485,7 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -149,7 +520,7 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
@@ -331,11 +702,537 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B6:N45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P43" sqref="P43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+    <col min="9" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C7" s="3"/>
+      <c r="D7" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+    </row>
+    <row r="8" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+    </row>
+    <row r="9" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="5">
+        <v>1</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="12" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+    </row>
+    <row r="13" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="18">
+        <v>600</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="17"/>
+    </row>
+    <row r="14" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="18">
+        <v>0</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="18">
+        <v>9</v>
+      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+    </row>
+    <row r="16" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="18">
+        <v>19</v>
+      </c>
+      <c r="E16" s="23"/>
+      <c r="F16" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="18">
+        <v>8</v>
+      </c>
+      <c r="E17" s="23"/>
+      <c r="F17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="17"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+    </row>
+    <row r="21" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+    </row>
+    <row r="22" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C22" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="33"/>
+    </row>
+    <row r="23" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C23" s="12"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+    </row>
+    <row r="24" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C24" s="24"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+    </row>
+    <row r="25" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C25" s="24"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+    </row>
+    <row r="26" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C26" s="24"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+    </row>
+    <row r="27" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C27" s="24"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+    </row>
+    <row r="28" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C28" s="24"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C29" s="24"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="25"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C30" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="34"/>
+    </row>
+    <row r="31" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="28"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+    </row>
+    <row r="32" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="28"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+    </row>
+    <row r="33" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C33" s="27"/>
+      <c r="D33" s="27"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="28"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="34" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="27"/>
+      <c r="H34" s="27"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+    </row>
+    <row r="35" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+    </row>
+    <row r="36" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+    </row>
+    <row r="37" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="28"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+    </row>
+    <row r="38" spans="3:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C38" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+    </row>
+    <row r="39" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
+      <c r="F39" s="35"/>
+      <c r="G39" s="35"/>
+      <c r="H39" s="35"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+    </row>
+    <row r="40" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="28"/>
+      <c r="K40" s="28"/>
+    </row>
+    <row r="41" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C41" s="35"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="35"/>
+      <c r="G41" s="35"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="36"/>
+      <c r="J41" s="28"/>
+      <c r="K41" s="28"/>
+    </row>
+    <row r="42" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C42" s="35"/>
+      <c r="D42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="36"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+    </row>
+    <row r="43" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+    </row>
+    <row r="44" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C44" s="35"/>
+      <c r="D44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+    </row>
+    <row r="45" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="35"/>
+      <c r="D45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="35"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="C43:H43"/>
+    <mergeCell ref="C44:H44"/>
+    <mergeCell ref="C45:H45"/>
+    <mergeCell ref="C36:H36"/>
+    <mergeCell ref="C37:H37"/>
+    <mergeCell ref="C38:K38"/>
+    <mergeCell ref="C39:H39"/>
+    <mergeCell ref="C40:H40"/>
+    <mergeCell ref="C41:H41"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C33:H33"/>
+    <mergeCell ref="C34:H34"/>
+    <mergeCell ref="C35:H35"/>
+    <mergeCell ref="C25:H25"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C30:K30"/>
+    <mergeCell ref="C21:K21"/>
+    <mergeCell ref="C22:K22"/>
+    <mergeCell ref="C23:H23"/>
+    <mergeCell ref="C24:H24"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:H16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C12:K12"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="D7:H7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>